<commit_message>
-used the tree algorithm -condition for weather feature -prediction is done
</commit_message>
<xml_diff>
--- a/Weatherdata.xlsx
+++ b/Weatherdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="30150" yWindow="510" windowWidth="17280" windowHeight="8820" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -412,13 +412,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="10.21875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10.109375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="59.44140625" bestFit="1" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -456,6 +461,11 @@
           <t>WindSpeed</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Condition</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -467,19 +477,24 @@
         <v>2022</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>285.27</v>
+        <v>21</v>
       </c>
       <c r="F2" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G2" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -492,19 +507,24 @@
         <v>2022</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>285.27</v>
+        <v>21</v>
       </c>
       <c r="F3" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G3" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -517,19 +537,24 @@
         <v>2022</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>285.27</v>
+        <v>30</v>
       </c>
       <c r="F4" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G4" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>['Hot', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -542,19 +567,24 @@
         <v>2022</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
       </c>
       <c r="E5" t="n">
-        <v>285.27</v>
+        <v>21</v>
       </c>
       <c r="F5" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G5" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -567,19 +597,24 @@
         <v>2022</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" t="n">
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>285.27</v>
+        <v>21</v>
       </c>
       <c r="F6" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G6" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -592,19 +627,24 @@
         <v>2022</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="n">
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>12.12</v>
+        <v>21</v>
       </c>
       <c r="F7" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G7" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -617,19 +657,24 @@
         <v>2022</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
         <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>12.12</v>
+        <v>29</v>
       </c>
       <c r="F8" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G8" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>['Hot', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -642,19 +687,24 @@
         <v>2022</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F9" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G9" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -667,19 +717,24 @@
         <v>2022</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F10" t="n">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="G10" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>['Cold', 'High Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -692,19 +747,24 @@
         <v>2022</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F11" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G11" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -717,19 +777,24 @@
         <v>2022</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
         <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F12" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G12" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>['Cold', 'High Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -742,19 +807,24 @@
         <v>2022</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F13" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G13" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -767,19 +837,24 @@
         <v>2022</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" t="n">
         <v>3</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14" t="n">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>1.03</v>
+        <v>10</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>['Cold', 'Low Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -792,19 +867,24 @@
         <v>2022</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" t="n">
         <v>3</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F15" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G15" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -817,19 +897,24 @@
         <v>2022</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="n">
         <v>3</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F16" t="n">
-        <v>82</v>
+        <v>37</v>
       </c>
       <c r="G16" t="n">
-        <v>1.03</v>
+        <v>6.17</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -842,19 +927,24 @@
         <v>2022</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="n">
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F17" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G17" t="n">
-        <v>1.54</v>
+        <v>6.17</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -867,19 +957,24 @@
         <v>2022</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="n">
         <v>3</v>
       </c>
       <c r="E18" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F18" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G18" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -892,19 +987,24 @@
         <v>2022</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
         <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F19" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G19" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -917,19 +1017,24 @@
         <v>2022</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="n">
         <v>3</v>
       </c>
       <c r="E20" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F20" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G20" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -942,19 +1047,24 @@
         <v>2022</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
         <v>3</v>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F21" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G21" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -967,19 +1077,24 @@
         <v>2022</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="n">
         <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F22" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G22" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -992,144 +1107,24 @@
         <v>2022</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
       </c>
       <c r="E23" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F23" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="G23" t="n">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Kathmandu</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" t="n">
-        <v>3</v>
-      </c>
-      <c r="E24" t="n">
-        <v>11</v>
-      </c>
-      <c r="F24" t="n">
-        <v>87</v>
-      </c>
-      <c r="G24" t="n">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Kathmandu</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="n">
-        <v>3</v>
-      </c>
-      <c r="E25" t="n">
-        <v>11</v>
-      </c>
-      <c r="F25" t="n">
-        <v>87</v>
-      </c>
-      <c r="G25" t="n">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Kathmandu</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" t="n">
-        <v>3</v>
-      </c>
-      <c r="E26" t="n">
-        <v>11</v>
-      </c>
-      <c r="F26" t="n">
-        <v>87</v>
-      </c>
-      <c r="G26" t="n">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Kathmandu</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" t="n">
-        <v>3</v>
-      </c>
-      <c r="E27" t="n">
-        <v>11</v>
-      </c>
-      <c r="F27" t="n">
-        <v>87</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Kathmandu</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="n">
-        <v>3</v>
-      </c>
-      <c r="E28" t="n">
-        <v>11</v>
-      </c>
-      <c r="F28" t="n">
-        <v>87</v>
-      </c>
-      <c r="G28" t="n">
-        <v>1.54</v>
+        <v>5.14</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-used the condition for the prediction
</commit_message>
<xml_diff>
--- a/Weatherdata.xlsx
+++ b/Weatherdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="30150" yWindow="510" windowWidth="17280" windowHeight="8820" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4512" yWindow="2172" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Temprature</t>
+          <t>Temp</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -477,10 +477,10 @@
         <v>2022</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>21</v>
@@ -493,7 +493,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+          <t>['Hot', 'High Humidity', 'High Wind']</t>
         </is>
       </c>
     </row>
@@ -627,23 +627,23 @@
         <v>2022</v>
       </c>
       <c r="C7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F7" t="n">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G7" t="n">
         <v>6.17</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+          <t>['Hot', 'Humidity', 'Low Wind']</t>
         </is>
       </c>
     </row>
@@ -1122,6 +1122,336 @@
         <v>5.14</v>
       </c>
       <c r="H23" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>3</v>
+      </c>
+      <c r="E24" t="n">
+        <v>23</v>
+      </c>
+      <c r="F24" t="n">
+        <v>27</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>3</v>
+      </c>
+      <c r="E25" t="n">
+        <v>23</v>
+      </c>
+      <c r="F25" t="n">
+        <v>27</v>
+      </c>
+      <c r="G25" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="n">
+        <v>23</v>
+      </c>
+      <c r="F26" t="n">
+        <v>27</v>
+      </c>
+      <c r="G26" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3</v>
+      </c>
+      <c r="E27" t="n">
+        <v>23</v>
+      </c>
+      <c r="F27" t="n">
+        <v>27</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" t="n">
+        <v>23</v>
+      </c>
+      <c r="F28" t="n">
+        <v>27</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" t="n">
+        <v>23</v>
+      </c>
+      <c r="F29" t="n">
+        <v>27</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" t="n">
+        <v>3</v>
+      </c>
+      <c r="E30" t="n">
+        <v>23</v>
+      </c>
+      <c r="F30" t="n">
+        <v>27</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" t="n">
+        <v>23</v>
+      </c>
+      <c r="F31" t="n">
+        <v>27</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" t="n">
+        <v>3</v>
+      </c>
+      <c r="E32" t="n">
+        <v>23</v>
+      </c>
+      <c r="F32" t="n">
+        <v>27</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E33" t="n">
+        <v>23</v>
+      </c>
+      <c r="F33" t="n">
+        <v>27</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Kathmandu</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2022</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E34" t="n">
+        <v>22</v>
+      </c>
+      <c r="F34" t="n">
+        <v>30</v>
+      </c>
+      <c r="G34" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="H34" t="inlineStr">
         <is>
           <t>['Cold', 'Mild Humidity', 'Low Wind']</t>
         </is>

</xml_diff>